<commit_message>
Finished Dr. Beex's edits and fixed cited works.
</commit_message>
<xml_diff>
--- a/Relevant Documents/Copy of Predicted Status Groups.xlsx
+++ b/Relevant Documents/Copy of Predicted Status Groups.xlsx
@@ -378,57 +378,7 @@
   <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr lIns="0" tIns="0" rIns="0" bIns="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" fontAlgn="auto" hangingPunct="1">
-              <a:lnSpc>
-                <a:spcPct val="100000"/>
-              </a:lnSpc>
-              <a:spcBef>
-                <a:spcPts val="0"/>
-              </a:spcBef>
-              <a:spcAft>
-                <a:spcPts val="0"/>
-              </a:spcAft>
-              <a:tabLst/>
-              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
-                <a:ea typeface=""/>
-                <a:cs typeface=""/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:uFillTx/>
-                <a:latin typeface="Calibri"/>
-                <a:ea typeface=""/>
-                <a:cs typeface=""/>
-              </a:rPr>
-              <a:t>Project Identification</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -439,7 +389,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Director Identification</c:v>
+            <c:v>Official Director</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -559,7 +509,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>PM Identification</c:v>
+            <c:v>Official PM</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -770,7 +720,8 @@
         <c:axId val="2104441760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1"/>
+          <c:max val="1.05"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -939,17 +890,8 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="t"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.14970638478402401"/>
-          <c:y val="9.4223274600108001E-2"/>
-          <c:w val="0.70058708939284298"/>
-          <c:h val="7.3211364441251703E-2"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1717,10 +1659,10 @@
     <xdr:from>
       <xdr:col>26</xdr:col>
       <xdr:colOff>402768</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>70756</xdr:rowOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>23811</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="8245932" cy="5161644"/>
+    <xdr:ext cx="8245932" cy="3632635"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -3091,8 +3033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="AJ60" sqref="AJ60"/>
+    <sheetView tabSelected="1" topLeftCell="D7" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="X34" sqref="X34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25"/>

</xml_diff>

<commit_message>
Worked through most of the small stuff today.  Gotta hit the big stuff tomorrow!
</commit_message>
<xml_diff>
--- a/Relevant Documents/Copy of Predicted Status Groups.xlsx
+++ b/Relevant Documents/Copy of Predicted Status Groups.xlsx
@@ -20,7 +20,7 @@
     <sheet name="outreach" sheetId="6" r:id="rId6"/>
     <sheet name="Operations" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -753,7 +753,7 @@
                     <a:spcPts val="0"/>
                   </a:spcAft>
                   <a:tabLst/>
-                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -763,7 +763,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" baseline="0">
+                  <a:rPr lang="en-US" sz="2200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" baseline="0">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -811,7 +811,7 @@
                 <a:spcPts val="0"/>
               </a:spcAft>
               <a:tabLst/>
-              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -863,7 +863,7 @@
                 <a:spcPts val="0"/>
               </a:spcAft>
               <a:tabLst/>
-              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -914,7 +914,7 @@
               <a:spcPts val="0"/>
             </a:spcAft>
             <a:tabLst/>
-            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:srgbClr val="595959"/>
               </a:solidFill>
@@ -1660,9 +1660,9 @@
       <xdr:col>26</xdr:col>
       <xdr:colOff>402768</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>23811</xdr:rowOff>
+      <xdr:rowOff>119061</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="8245932" cy="3632635"/>
+    <xdr:ext cx="8122106" cy="3537385"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -3033,8 +3033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D7" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="X34" sqref="X34"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="AK44" sqref="AK44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25"/>

</xml_diff>